<commit_message>
feat: Add 'Add Lists' feature to shopping list and update UI components
</commit_message>
<xml_diff>
--- a/import/recipes.xlsx
+++ b/import/recipes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mheyi\Projects\HeyinkMeals\import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CF2D2D8D-3F1A-4C7C-80E6-9C4F40D5E001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A85FB0B6-034A-4FE4-9890-CA76BF23F935}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{396531AE-A036-475C-A2F5-829993F4DACA}"/>
   </bookViews>
@@ -323,17 +323,18 @@
       <sheetName val="grocery_categories"/>
       <sheetName val="grocery_types"/>
       <sheetName val="grocery_lists"/>
+      <sheetName val="grocery_list_items"/>
       <sheetName val="recipes"/>
-      <sheetName val="grocery_list_items"/>
       <sheetName val="Sheet8"/>
       <sheetName val="Sheet1"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4">
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5">
         <row r="1">
           <cell r="B1" t="str">
             <v>instructions</v>
@@ -355,7 +356,6 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="5"/>
       <sheetData sheetId="6">
         <row r="1">
           <cell r="B1" t="str">
@@ -2414,7 +2414,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="7"/>
+      <sheetData sheetId="7" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2793,27 +2793,27 @@
         <v>3</v>
       </c>
       <c r="B4" t="str">
-        <f ca="1">VLOOKUP($A4,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A4,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v/>
       </c>
       <c r="C4">
-        <f ca="1">VLOOKUP($A4,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A4,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>2</v>
       </c>
       <c r="D4">
-        <f ca="1">VLOOKUP($A4,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A4,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="E4">
-        <f ca="1">VLOOKUP($A4,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A4,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="F4">
-        <f ca="1">VLOOKUP($A4,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A4,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>5</v>
       </c>
       <c r="G4" t="str">
-        <f ca="1">VLOOKUP($A4,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A4,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v/>
       </c>
     </row>
@@ -2822,29 +2822,29 @@
         <v>4</v>
       </c>
       <c r="B5" t="str">
-        <f ca="1">VLOOKUP($A5,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A5,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>Warm meal.
 Make rice.
 Fry paratas in a small amount of buter.</v>
       </c>
       <c r="C5">
-        <f ca="1">VLOOKUP($A5,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A5,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>3</v>
       </c>
       <c r="D5">
-        <f ca="1">VLOOKUP($A5,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A5,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="E5">
-        <f ca="1">VLOOKUP($A5,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A5,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="F5">
-        <f ca="1">VLOOKUP($A5,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A5,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>30</v>
       </c>
       <c r="G5" t="str">
-        <f ca="1">VLOOKUP($A5,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A5,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v/>
       </c>
     </row>
@@ -2853,30 +2853,30 @@
         <v>5</v>
       </c>
       <c r="B6" t="str">
-        <f ca="1">VLOOKUP($A6,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A6,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>1. Clean sweetcorn.
 2. Boil in salted water.
 3. Char on the braai.
 4. Brush with melted butter and top with chipotle spice and a squeeze of lime.</v>
       </c>
       <c r="C6">
-        <f ca="1">VLOOKUP($A6,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A6,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>4</v>
       </c>
       <c r="D6">
-        <f ca="1">VLOOKUP($A6,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A6,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="E6">
-        <f ca="1">VLOOKUP($A6,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A6,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="F6">
-        <f ca="1">VLOOKUP($A6,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A6,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>20</v>
       </c>
       <c r="G6" t="str">
-        <f ca="1">VLOOKUP($A6,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A6,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v/>
       </c>
     </row>
@@ -2885,7 +2885,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="str">
-        <f ca="1">VLOOKUP($A7,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A7,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>1. Preheat oven to 220 C.
 2. Add your rinsed, drained and dried chickpeas on a baking sheet lined with parchment paper.
 3. Bake for 30-35 minutes or until crunchy and golden brown. Do not burn!
@@ -2897,23 +2897,23 @@
 (Store in fridge or freezer.)</v>
       </c>
       <c r="C7">
-        <f ca="1">VLOOKUP($A7,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A7,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>10</v>
       </c>
       <c r="D7">
-        <f ca="1">VLOOKUP($A7,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A7,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="E7">
-        <f ca="1">VLOOKUP($A7,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A7,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="F7">
-        <f ca="1">VLOOKUP($A7,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A7,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>45</v>
       </c>
       <c r="G7" t="str">
-        <f ca="1">VLOOKUP($A7,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A7,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>https://healthygirlkitchen.com/recipes/vegan-chocolate-chickpea-bark-oil-free/</v>
       </c>
     </row>
@@ -2922,30 +2922,30 @@
         <v>7</v>
       </c>
       <c r="B8" t="str">
-        <f ca="1">VLOOKUP($A8,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A8,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>1. Preheat the grill.
 2. Grease a baking tray and arrange the frozen hake fillets on the tray.
 3. Season with salt, pepper and add a large knob of butter.
 4. Grill for 5–7 minutes.</v>
       </c>
       <c r="C8">
-        <f ca="1">VLOOKUP($A8,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A8,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>2</v>
       </c>
       <c r="D8">
-        <f ca="1">VLOOKUP($A8,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A8,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="E8">
-        <f ca="1">VLOOKUP($A8,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A8,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="F8">
-        <f ca="1">VLOOKUP($A8,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A8,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>10</v>
       </c>
       <c r="G8" t="str">
-        <f ca="1">VLOOKUP($A8,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A8,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v/>
       </c>
     </row>
@@ -2954,27 +2954,27 @@
         <v>8</v>
       </c>
       <c r="B9" t="str">
-        <f ca="1">VLOOKUP($A9,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A9,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v/>
       </c>
       <c r="C9">
-        <f ca="1">VLOOKUP($A9,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A9,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>4</v>
       </c>
       <c r="D9">
-        <f ca="1">VLOOKUP($A9,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A9,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="E9">
-        <f ca="1">VLOOKUP($A9,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A9,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="F9" t="str">
-        <f ca="1">VLOOKUP($A9,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A9,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v/>
       </c>
       <c r="G9" t="str">
-        <f ca="1">VLOOKUP($A9,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A9,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v/>
       </c>
     </row>
@@ -2983,30 +2983,30 @@
         <v>9</v>
       </c>
       <c r="B10" t="str">
-        <f ca="1">VLOOKUP($A10,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A10,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>1. Dish half a cup of yoghurt into a bowl.
 2. Peel and grate the mango (which should be frozen).
 3. Grate some lime/lemon zest.
 4. Add chopped chocolate and mint with some cubed mango.</v>
       </c>
       <c r="C10" t="str">
-        <f ca="1">VLOOKUP($A10,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A10,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v/>
       </c>
       <c r="D10">
-        <f ca="1">VLOOKUP($A10,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A10,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="E10">
-        <f ca="1">VLOOKUP($A10,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A10,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="F10" t="str">
-        <f ca="1">VLOOKUP($A10,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A10,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v/>
       </c>
       <c r="G10" t="str">
-        <f ca="1">VLOOKUP($A10,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A10,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>https://www.instagram.com/p/C3aez42Nf9R/</v>
       </c>
     </row>
@@ -3015,30 +3015,30 @@
         <v>10</v>
       </c>
       <c r="B11" t="str">
-        <f ca="1">VLOOKUP($A11,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A11,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>1. Warm milk in nutribullet cup for 2 mins.
 2. Add other ingredients.
 3. Mix in nutribullet.
 4. Heat again in microwave in 30sec increments (about 4 times).</v>
       </c>
       <c r="C11">
-        <f ca="1">VLOOKUP($A11,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A11,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>2</v>
       </c>
       <c r="D11">
-        <f ca="1">VLOOKUP($A11,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A11,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="E11">
-        <f ca="1">VLOOKUP($A11,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A11,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="F11">
-        <f ca="1">VLOOKUP($A11,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A11,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>10</v>
       </c>
       <c r="G11" t="str">
-        <f ca="1">VLOOKUP($A11,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A11,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>https://www.theconsciousplantkitchen.com/vegan-hot-chocolate/</v>
       </c>
     </row>
@@ -3047,7 +3047,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="str">
-        <f ca="1">VLOOKUP($A12,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A12,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>Pour coconut oil and honey into a heatproof bowl.
 Microwave for about 40 seconds, until the coconut
 oil is completely melted.
@@ -3061,23 +3061,23 @@
 chocolate.</v>
       </c>
       <c r="C12" t="str">
-        <f ca="1">VLOOKUP($A12,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A12,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v/>
       </c>
       <c r="D12">
-        <f ca="1">VLOOKUP($A12,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A12,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="E12">
-        <f ca="1">VLOOKUP($A12,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A12,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="F12" t="str">
-        <f ca="1">VLOOKUP($A12,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A12,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v/>
       </c>
       <c r="G12" t="str">
-        <f ca="1">VLOOKUP($A12,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A12,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>https://www.cocobeancooks.com/post/peanut-butter-freezer-fudge</v>
       </c>
     </row>
@@ -3086,7 +3086,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="str">
-        <f ca="1">VLOOKUP($A13,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A13,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>1. Add butter to a frying pain and saute almonds until golden.
 2. Then add mushrooms, the juice of half a lemon, 2T parsley, salt and pepper.
 3. Cook gently over low heat until mushrooms are tender.
@@ -3094,23 +3094,23 @@
 5. Serve over fish with a sprinkle of parsley on top.</v>
       </c>
       <c r="C13">
-        <f ca="1">VLOOKUP($A13,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A13,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>6</v>
       </c>
       <c r="D13">
-        <f ca="1">VLOOKUP($A13,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A13,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="E13">
-        <f ca="1">VLOOKUP($A13,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A13,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="F13" t="str">
-        <f ca="1">VLOOKUP($A13,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A13,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v/>
       </c>
       <c r="G13" t="str">
-        <f ca="1">VLOOKUP($A13,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A13,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v/>
       </c>
     </row>
@@ -3119,7 +3119,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="str">
-        <f ca="1">VLOOKUP($A14,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A14,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>1. In a large pot over medium heat, bring 3L of heavily salted water to a boil. Have a large bowl of ice water ready on the side.
 2. Add the broccolini and cook for 2 to 3 minutes, depending on the size of the broccolini. Quickly drain the water and place the broccolini in the ice bath to stop the cooking process. When the broccolini is cool remove them from the ice bath and place on a paper towel- lined plate.
 3. Preheat the oven to broil with a rack set in the top third of the oven. In a medium bowl toss the broccolini in olive oil, shallot, garlic to coat then arrange in a single even layer on a baking sheet.
@@ -3127,23 +3127,23 @@
 5. Remove from the broiler and place back in the bowl. Add the red wine vinegar and chili oil and serve.</v>
       </c>
       <c r="C14">
-        <f ca="1">VLOOKUP($A14,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A14,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>4</v>
       </c>
       <c r="D14">
-        <f ca="1">VLOOKUP($A14,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A14,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="E14">
-        <f ca="1">VLOOKUP($A14,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A14,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="F14">
-        <f ca="1">VLOOKUP($A14,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A14,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>15</v>
       </c>
       <c r="G14" t="str">
-        <f ca="1">VLOOKUP($A14,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A14,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>https://whatsgabycooking.com/the-best-chili-garlic-broccolini/</v>
       </c>
     </row>
@@ -3152,30 +3152,30 @@
         <v>14</v>
       </c>
       <c r="B15" t="str">
-        <f ca="1">VLOOKUP($A15,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A15,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>1. Blend drained chickpeas with pesto.
 2. Spread chickpea pesto on the bread.
 3. Top one side of the sandwich with rocket, artichoke and avocado.
 4. Put other half of bread on top and toast in a press.</v>
       </c>
       <c r="C15">
-        <f ca="1">VLOOKUP($A15,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A15,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>2</v>
       </c>
       <c r="D15">
-        <f ca="1">VLOOKUP($A15,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A15,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="E15">
-        <f ca="1">VLOOKUP($A15,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A15,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="F15">
-        <f ca="1">VLOOKUP($A15,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A15,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>10</v>
       </c>
       <c r="G15" t="str">
-        <f ca="1">VLOOKUP($A15,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A15,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v/>
       </c>
     </row>
@@ -3184,7 +3184,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="str">
-        <f ca="1">VLOOKUP($A16,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A16,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>Place ingredients on a baking tray (except coconut flakes).
 Cover with honey.
 Bake until golden.
@@ -3192,23 +3192,23 @@
 Combine coconut flakes.</v>
       </c>
       <c r="C16" t="str">
-        <f ca="1">VLOOKUP($A16,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A16,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v/>
       </c>
       <c r="D16">
-        <f ca="1">VLOOKUP($A16,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A16,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="E16">
-        <f ca="1">VLOOKUP($A16,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A16,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="F16" t="str">
-        <f ca="1">VLOOKUP($A16,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A16,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v/>
       </c>
       <c r="G16" t="str">
-        <f ca="1">VLOOKUP($A16,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A16,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v/>
       </c>
     </row>
@@ -3217,7 +3217,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="str">
-        <f ca="1">VLOOKUP($A17,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A17,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v xml:space="preserve">Preheat the oven to 180°C. Line a baking tray with baking paper.
 Arrange the pumpkin pieces on the baking tray. Drizzle with 2 tablespoons olive oil and season with sea salt and pepper. Place the tray in the oven to roast for 25 minutes.
 Whilst the pumpkin is roasting, heat the remaining olive oil in a non-stick frying pan over a medium heat. Add the sliced onion to the pan and cook for 6-7 minutes until softened. Add the balsamic vinegar and coconut sugar and stir to coat. Reduce the heat slightly and cook for a further 7-8 minutes or until the onion is golden and caramelised.
@@ -3228,23 +3228,23 @@
 Makes: 6-8 slices </v>
       </c>
       <c r="C17">
-        <f ca="1">VLOOKUP($A17,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A17,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>4</v>
       </c>
       <c r="D17">
-        <f ca="1">VLOOKUP($A17,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A17,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="E17">
-        <f ca="1">VLOOKUP($A17,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A17,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="F17" t="str">
-        <f ca="1">VLOOKUP($A17,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A17,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v/>
       </c>
       <c r="G17" t="str">
-        <f ca="1">VLOOKUP($A17,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A17,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>https://www.instagram.com/p/C3qXj-zSiM8/</v>
       </c>
     </row>
@@ -3253,7 +3253,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="str">
-        <f ca="1">VLOOKUP($A18,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A18,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>1. Grate parmesan.
 2. Toast pine nutes.
 3. Pour 2 cups of peas into a glass measuring cup/glass bowl and cover the peas with water. Microwave the peas for 2 minutes, strain and then place the peas into your food processor/blender.
@@ -3262,23 +3262,23 @@
 6. Serve immediately with Parmesan Pea Purée, toasted pine nuts, mint leaves (if desired) and more Parmesan cheese (if desired).</v>
       </c>
       <c r="C18">
-        <f ca="1">VLOOKUP($A18,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A18,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>2</v>
       </c>
       <c r="D18">
-        <f ca="1">VLOOKUP($A18,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A18,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="E18">
-        <f ca="1">VLOOKUP($A18,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A18,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="F18">
-        <f ca="1">VLOOKUP($A18,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A18,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>30</v>
       </c>
       <c r="G18" t="str">
-        <f ca="1">VLOOKUP($A18,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A18,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>https://www.healthylittlevittles.com/crispy-cauliflower-gnocchi-with-parmesan-pea-puree/</v>
       </c>
     </row>
@@ -3287,7 +3287,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="str">
-        <f ca="1">VLOOKUP($A19,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A19,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>1. Whisk together the cocoa powder, espresso and vanilla in a bowl and set aside
 2. In a mixer or using a hand mixer, beat the egg yolks and sugar until pale and thick, about 5 minutes.
 3. Add in the salt, mascarpone cheese and continue to whip until smooth.
@@ -3299,23 +3299,23 @@
 9. Cover with plastic wrap and chill for at least 2 hours before serving.</v>
       </c>
       <c r="C19">
-        <f ca="1">VLOOKUP($A19,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A19,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>8</v>
       </c>
       <c r="D19">
-        <f ca="1">VLOOKUP($A19,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A19,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="E19">
-        <f ca="1">VLOOKUP($A19,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A19,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="F19">
-        <f ca="1">VLOOKUP($A19,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A19,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>15</v>
       </c>
       <c r="G19" t="str">
-        <f ca="1">VLOOKUP($A19,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A19,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>https://whatsgabycooking.com/classic-italian-tiramisu/</v>
       </c>
     </row>
@@ -3324,7 +3324,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="str">
-        <f ca="1">VLOOKUP($A20,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A20,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>Place a medium, saucepan over a medium/high heat, add the olive oil leek, garlic, and a good pinch of salt. Cook this stirring for 4-5 minutes, stirring often.
 Add the baby spinach, peas and cook another 2 minutes, to wilt the spinach and defrost the peas.
 Transfer ¾ of the veggie mix to a blender, keep the remainder in the pot, set aside.
@@ -3335,23 +3335,23 @@
 Season to taste and serve, topped with remaining cottage cheese and a crack of black pepper.</v>
       </c>
       <c r="C20">
-        <f ca="1">VLOOKUP($A20,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A20,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>4</v>
       </c>
       <c r="D20">
-        <f ca="1">VLOOKUP($A20,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A20,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="E20">
-        <f ca="1">VLOOKUP($A20,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A20,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="F20" t="str">
-        <f ca="1">VLOOKUP($A20,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A20,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v/>
       </c>
       <c r="G20" t="str">
-        <f ca="1">VLOOKUP($A20,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A20,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>https://www.instagram.com/p/DDJuFm1Srq8/</v>
       </c>
     </row>
@@ -3360,27 +3360,27 @@
         <v>20</v>
       </c>
       <c r="B21" t="str">
-        <f ca="1">VLOOKUP($A21,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A21,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v/>
       </c>
       <c r="C21">
-        <f ca="1">VLOOKUP($A21,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A21,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>2</v>
       </c>
       <c r="D21">
-        <f ca="1">VLOOKUP($A21,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A21,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="E21">
-        <f ca="1">VLOOKUP($A21,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A21,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="F21" t="str">
-        <f ca="1">VLOOKUP($A21,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A21,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v/>
       </c>
       <c r="G21" t="str">
-        <f ca="1">VLOOKUP($A21,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A21,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v/>
       </c>
     </row>
@@ -3389,7 +3389,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="str">
-        <f ca="1">VLOOKUP($A22,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A22,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>Soak cashews for 3 hours.
 Steam pumpkin and cauliflower.
 Cook pasta.
@@ -3397,23 +3397,23 @@
 Combine sauce and pasta.</v>
       </c>
       <c r="C22">
-        <f ca="1">VLOOKUP($A22,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A22,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>2</v>
       </c>
       <c r="D22">
-        <f ca="1">VLOOKUP($A22,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A22,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="E22">
-        <f ca="1">VLOOKUP($A22,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A22,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="F22" t="str">
-        <f ca="1">VLOOKUP($A22,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A22,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v/>
       </c>
       <c r="G22" t="str">
-        <f ca="1">VLOOKUP($A22,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A22,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v/>
       </c>
     </row>
@@ -3422,7 +3422,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="str">
-        <f ca="1">VLOOKUP($A23,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A23,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>1. Preheat the oven to 180°C. Line a loaf tin with tin foil and grease the foil-lined tin.
 2. Beat the butter and sugar together until pale and creamy.
 3. Add the mashed bananas and beat until well combined.
@@ -3433,23 +3433,23 @@
 8. Serve fresh out of the oven, as is or with lots of butter. Freeze and then toast and top with a blob of marscapone and some toasted pecan nuts or cocoa nibs.</v>
       </c>
       <c r="C23">
-        <f ca="1">VLOOKUP($A23,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A23,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>1</v>
       </c>
       <c r="D23">
-        <f ca="1">VLOOKUP($A23,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A23,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="E23">
-        <f ca="1">VLOOKUP($A23,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A23,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="F23" t="str">
-        <f ca="1">VLOOKUP($A23,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A23,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v/>
       </c>
       <c r="G23" t="str">
-        <f ca="1">VLOOKUP($A23,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A23,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>http://Delish Sisters</v>
       </c>
     </row>
@@ -3458,30 +3458,30 @@
         <v>23</v>
       </c>
       <c r="B24" t="str">
-        <f ca="1">VLOOKUP($A24,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A24,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>1. Cook the linguine in a saucepan of salted boiling water for about 10 minutes until al dente, adding the peas after 8 minutes.
 2. Meanwhile, heat the oil in a large saucepan or frying pan over a medium heat and fry the garlic with the chilli flakes for 30 seconds, without colouring.
 3. Add the prawns and toss in the garlic. Stir in the mascarpone, rocket, lemon zest and juice and heat for a minute or so, or until the rocket wilts.
 4. Drain the pasta and peas, add to the sauce and mix together. Season with salt and pepper. Make sure that the prawns, rocket and peas are evenly distributed before serving.</v>
       </c>
       <c r="C24">
-        <f ca="1">VLOOKUP($A24,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A24,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>4</v>
       </c>
       <c r="D24">
-        <f ca="1">VLOOKUP($A24,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A24,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="E24">
-        <f ca="1">VLOOKUP($A24,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A24,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="F24">
-        <f ca="1">VLOOKUP($A24,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A24,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>20</v>
       </c>
       <c r="G24" t="str">
-        <f ca="1">VLOOKUP($A24,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A24,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>https://www.bbc.co.uk/food/recipes/prawn_linguine_02687</v>
       </c>
     </row>
@@ -3490,7 +3490,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="str">
-        <f ca="1">VLOOKUP($A25,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A25,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>Preheat the oven to 200C.
 In a shallow casserole dish, heat some olive oil and gently saute your sliced garlic until it's starting to brown.
 Add the smoked paprika and oregano and stir for a moment until fragrant, then add the tomatoes, sugar and red wine vinegar.
@@ -3502,23 +3502,23 @@
 halloumi browned on top, turn on the grill / broiler for the last 5 minutes.</v>
       </c>
       <c r="C25">
-        <f ca="1">VLOOKUP($A25,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A25,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>4</v>
       </c>
       <c r="D25">
-        <f ca="1">VLOOKUP($A25,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A25,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="E25">
-        <f ca="1">VLOOKUP($A25,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A25,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="F25">
-        <f ca="1">VLOOKUP($A25,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A25,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>35</v>
       </c>
       <c r="G25" t="str">
-        <f ca="1">VLOOKUP($A25,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A25,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>https://www.happyveggiekitchen.com/halloumi-bake/#recipe</v>
       </c>
     </row>
@@ -3527,27 +3527,27 @@
         <v>25</v>
       </c>
       <c r="B26" t="str">
-        <f ca="1">VLOOKUP($A26,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A26,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v/>
       </c>
       <c r="C26" t="str">
-        <f ca="1">VLOOKUP($A26,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A26,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v/>
       </c>
       <c r="D26">
-        <f ca="1">VLOOKUP($A26,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A26,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="E26">
-        <f ca="1">VLOOKUP($A26,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A26,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="F26" t="str">
-        <f ca="1">VLOOKUP($A26,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A26,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v/>
       </c>
       <c r="G26" t="str">
-        <f ca="1">VLOOKUP($A26,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A26,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>https://fashionablehostess.com/winter-white-cheese-board/</v>
       </c>
     </row>
@@ -3556,7 +3556,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="str">
-        <f ca="1">VLOOKUP($A27,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A27,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>1. Defrost the prawns by thawing and then get rid of excess water - Marinate the prawns with the birds eye chilli, garlic, zest and juice of 1 lemon and salt. Refrigerate for 30 minutes
 2. Boil pasta in salted water as per instructions on the packet. Cook until al la dente, drain the water. Reserve some of the pasta water to add to the final dish.
 3. Heat one tablespoon butter, with a few drops of oil, in a pan and flash fry half the prawns in 2, 30 seconds on each side. Add another tablespoon of butter and fry remaining prawns. Transfer to a bowl and set aside
@@ -3565,23 +3565,23 @@
 6. Divide pasta into pasta bowls and add the prawn sauce on top. Garnish with parsley and add some parmesan if you like.</v>
       </c>
       <c r="C27">
-        <f ca="1">VLOOKUP($A27,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A27,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>2</v>
       </c>
       <c r="D27">
-        <f ca="1">VLOOKUP($A27,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A27,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="E27">
-        <f ca="1">VLOOKUP($A27,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A27,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="F27" t="str">
-        <f ca="1">VLOOKUP($A27,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A27,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v/>
       </c>
       <c r="G27" t="str">
-        <f ca="1">VLOOKUP($A27,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A27,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>https://www.instagram.com/p/C5QYDb8MHzB/</v>
       </c>
     </row>
@@ -3590,7 +3590,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="str">
-        <f ca="1">VLOOKUP($A28,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A28,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>1. Cook the sweet potato and set aside . 
 2. Add the chili powder to the rinsed black beans and then heat them up on the stove top for a few minutes until hot. 
 3. Cut the sweet potato in half and open it up slightly to fit your other ingredients. 
@@ -3598,23 +3598,23 @@
 5. Top the sweet potato with the black beans, sour cream, salsa and guacamole.</v>
       </c>
       <c r="C28">
-        <f ca="1">VLOOKUP($A28,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A28,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>2</v>
       </c>
       <c r="D28">
-        <f ca="1">VLOOKUP($A28,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A28,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="E28">
-        <f ca="1">VLOOKUP($A28,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A28,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="F28" t="str">
-        <f ca="1">VLOOKUP($A28,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A28,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v/>
       </c>
       <c r="G28" t="str">
-        <f ca="1">VLOOKUP($A28,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A28,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>https://healthygirlkitchen.com/recipes/mexican-stuffed-sweet-potatoes-vegan-oil-free/</v>
       </c>
     </row>
@@ -3623,7 +3623,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="str">
-        <f ca="1">VLOOKUP($A29,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A29,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>1. Cook pasta. While pasta is boiling, get a large non-stick pan and start sauteing the zucchini.
 2. Saute zucchini in a little water or avocado/olive oil, your choice. Saute until tender but not too mushy.
 3. Add artichokes to pan, just dump the whole jar in there!
@@ -3633,23 +3633,23 @@
 7. Serve and enjoy!</v>
       </c>
       <c r="C29">
-        <f ca="1">VLOOKUP($A29,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A29,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>4</v>
       </c>
       <c r="D29">
-        <f ca="1">VLOOKUP($A29,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A29,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="E29">
-        <f ca="1">VLOOKUP($A29,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A29,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="F29" t="str">
-        <f ca="1">VLOOKUP($A29,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A29,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v/>
       </c>
       <c r="G29" t="str">
-        <f ca="1">VLOOKUP($A29,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A29,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>https://healthygirlkitchen.com/recipes/vegan-mediterranean-pasta/</v>
       </c>
     </row>
@@ -3658,7 +3658,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="str">
-        <f ca="1">VLOOKUP($A30,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A30,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>1. Make couscous (2c)
 2. Steam peas (1c).
 3. Dice and saute zucchini in olive oil, salt and pepper.
@@ -3667,23 +3667,23 @@
 6. Top with salt, pepper and lemon juice.</v>
       </c>
       <c r="C30">
-        <f ca="1">VLOOKUP($A30,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A30,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>4</v>
       </c>
       <c r="D30">
-        <f ca="1">VLOOKUP($A30,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A30,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="E30">
-        <f ca="1">VLOOKUP($A30,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A30,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="F30">
-        <f ca="1">VLOOKUP($A30,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A30,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>10</v>
       </c>
       <c r="G30" t="str">
-        <f ca="1">VLOOKUP($A30,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A30,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>https://www.instagram.com/p/CgiO2F7Jfe5/</v>
       </c>
     </row>
@@ -3692,29 +3692,29 @@
         <v>30</v>
       </c>
       <c r="B31" t="str">
-        <f ca="1">VLOOKUP($A31,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A31,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>1. Preheat the oven to 200° C.
 2. In a 23×33 cm baking dish, combine the olive oil, garlic, onion, basil, paprika, chili flakes, salt, and pepper. Add the dry orzo, artichokes, and pesto. Pour over 2 1/4 cups of water and stir to combine. Place the spinach on top. Bake for 12-15 minutes, until most of the water has cooked into the pasta, but not all of it.
 3. Stir the pasta around, then sprinkle the cheeses overtop. Bake another 10 minutes, until the cheese has melted and the sauce is bubbling. If there's a lot of oil from the pesto on top, drain off the excess. Top with fresh basil!</v>
       </c>
       <c r="C31">
-        <f ca="1">VLOOKUP($A31,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A31,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>6</v>
       </c>
       <c r="D31">
-        <f ca="1">VLOOKUP($A31,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A31,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="E31">
-        <f ca="1">VLOOKUP($A31,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A31,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="F31">
-        <f ca="1">VLOOKUP($A31,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A31,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>35</v>
       </c>
       <c r="G31" t="str">
-        <f ca="1">VLOOKUP($A31,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A31,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>https://www.halfbakedharvest.com/spinach-and-artichoke-orzo-bake/</v>
       </c>
     </row>
@@ -3723,7 +3723,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="str">
-        <f ca="1">VLOOKUP($A32,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A32,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>1. Toast and crush fennel seeds.
 2. In a medium bowl, mix the feta (broken into 1-2cm pieces) with a quarter-teaspoon of the chilli flakes, 1 teaspoon of the fennel seeds and a tablespoon of oil. Set aside while you cook the orzo.
 3. Put a large saute pan for which you have a lid on a medium-high heat. Add two tablespoons of oil, the orzo, an eighth of a teaspoon of salt and a good grind of pepper. Fry for three to four minutes, stirring frequently, until golden brown, then remove from the pan and set aside.
@@ -3733,23 +3733,23 @@
 7. Stir in the basil and serve at once with the marinated feta sprinkled on top.</v>
       </c>
       <c r="C32">
-        <f ca="1">VLOOKUP($A32,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A32,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>4</v>
       </c>
       <c r="D32">
-        <f ca="1">VLOOKUP($A32,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A32,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="E32">
-        <f ca="1">VLOOKUP($A32,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A32,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="F32">
-        <f ca="1">VLOOKUP($A32,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A32,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>45</v>
       </c>
       <c r="G32" t="str">
-        <f ca="1">VLOOKUP($A32,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A32,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>https://www.theguardian.com/food/2018/sep/01/easy-does-it-seven-simple-yotam-ottolenghi-recipes?page=with%3Aimg-4#img-4</v>
       </c>
     </row>
@@ -3758,7 +3758,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="str">
-        <f ca="1">VLOOKUP($A33,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A33,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>Fry capers, anchovy fillets, chopped garlic, halved olives and chopped chilli in 2 T olive oil in a large ovenproof pan over a medium to low heat.
 When fragrant, add the cherry tomatoes and bring to a simmer. Add tomato paste and a little water if necessary to loosen.
 Meanwhile preheat the grill, grease a baking tray and arrange the frozen hake fillets on the tray. Season and grill for 5–7 minutes. Place thefish in the sauce and grate over Parmesan, then grill until golden and bubbling, 3–5 minutes.
@@ -3766,23 +3766,23 @@
 Cook's note: The worst thing about entertaining? Washing up, hands down. Do yourself a favour and serve this winning supper in the centre of the table, straight out the pan</v>
       </c>
       <c r="C33">
-        <f ca="1">VLOOKUP($A33,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A33,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>4</v>
       </c>
       <c r="D33">
-        <f ca="1">VLOOKUP($A33,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A33,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="E33">
-        <f ca="1">VLOOKUP($A33,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A33,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="F33">
-        <f ca="1">VLOOKUP($A33,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A33,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>25</v>
       </c>
       <c r="G33" t="str">
-        <f ca="1">VLOOKUP($A33,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A33,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>https://taste.co.za/recipes/puttanesca-baked-fish/</v>
       </c>
     </row>
@@ -3791,7 +3791,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="str">
-        <f ca="1">VLOOKUP($A34,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A34,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>Preheat oven 200C.
 Line heavy duty foil with greaseproof paper.
 Combine dressing ingredients.
@@ -3801,23 +3801,23 @@
 Serve.</v>
       </c>
       <c r="C34">
-        <f ca="1">VLOOKUP($A34,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A34,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>2</v>
       </c>
       <c r="D34">
-        <f ca="1">VLOOKUP($A34,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A34,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="E34">
-        <f ca="1">VLOOKUP($A34,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A34,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="F34">
-        <f ca="1">VLOOKUP($A34,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A34,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>20</v>
       </c>
       <c r="G34" t="str">
-        <f ca="1">VLOOKUP($A34,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A34,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v/>
       </c>
     </row>
@@ -3826,7 +3826,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="str">
-        <f ca="1">VLOOKUP($A35,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A35,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>Step 1
 Place one third of the cashews into a food
 processor and pulse for a few seconds until
@@ -3849,23 +3849,23 @@
 courgetti) and sprinkle with the toasted cashews.</v>
       </c>
       <c r="C35">
-        <f ca="1">VLOOKUP($A35,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A35,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>2</v>
       </c>
       <c r="D35">
-        <f ca="1">VLOOKUP($A35,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A35,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="E35">
-        <f ca="1">VLOOKUP($A35,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A35,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="F35">
-        <f ca="1">VLOOKUP($A35,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A35,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>15</v>
       </c>
       <c r="G35" t="str">
-        <f ca="1">VLOOKUP($A35,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A35,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v/>
       </c>
     </row>
@@ -3874,30 +3874,30 @@
         <v>35</v>
       </c>
       <c r="B36" t="str">
-        <f ca="1">VLOOKUP($A36,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A36,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>1. Preheat the oven to 425° F. Line a baking sheet with parchment paper.
 2. in a bowl, toss together the olive oil, tomatoes, thyme, oregano, garlic, chili flakes, salt, and pepper.
 3. Cut each sheet of puff pastry into 4 squares. Spread each square with a tablespoons of pesto, leaving a 1/2 inch border. Sprinkle the cheese over the pesto. Arrange the tomatoes over the cheese.
 4. Fold the edges of the pastry inward to enclose. Bake 15-20 minutes, until the pastry is golden and the cheese has melted. Break the burrata over the warm tomatoes, then spoon over the pesto. Top with fresh basil. Enjoy!</v>
       </c>
       <c r="C36">
-        <f ca="1">VLOOKUP($A36,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A36,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>8</v>
       </c>
       <c r="D36">
-        <f ca="1">VLOOKUP($A36,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A36,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="E36">
-        <f ca="1">VLOOKUP($A36,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A36,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="F36">
-        <f ca="1">VLOOKUP($A36,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A36,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>30</v>
       </c>
       <c r="G36" t="str">
-        <f ca="1">VLOOKUP($A36,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A36,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>https://www.halfbakedharvest.com/caprese-pesto-tarts/</v>
       </c>
     </row>
@@ -3906,7 +3906,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="str">
-        <f ca="1">VLOOKUP($A37,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A37,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>1. Finely chop onion, garlic and chilli and grate mushrooms and carrots.
 2. Saute onion, garlic and chilli until softened.
 3. Add grated mushrooms and carrots, and fry for 10 minutes.
@@ -3917,23 +3917,23 @@
 8. Combine and serve with grated parmesean.</v>
       </c>
       <c r="C37">
-        <f ca="1">VLOOKUP($A37,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A37,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>4</v>
       </c>
       <c r="D37">
-        <f ca="1">VLOOKUP($A37,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A37,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="E37">
-        <f ca="1">VLOOKUP($A37,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A37,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="F37">
-        <f ca="1">VLOOKUP($A37,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A37,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>40</v>
       </c>
       <c r="G37" t="str">
-        <f ca="1">VLOOKUP($A37,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A37,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v/>
       </c>
     </row>
@@ -3942,7 +3942,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="str">
-        <f ca="1">VLOOKUP($A38,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A38,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>STEP 1
 Prepare ingredients:
 - toast almonds
@@ -3958,23 +3958,23 @@
 Arrange the halloumi on the plate and finish with the pesto, olive oil, lemon juice, and herbs for garnish. Serve while the halloumi is warm.</v>
       </c>
       <c r="C38">
-        <f ca="1">VLOOKUP($A38,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A38,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>4</v>
       </c>
       <c r="D38">
-        <f ca="1">VLOOKUP($A38,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A38,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="E38">
-        <f ca="1">VLOOKUP($A38,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A38,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="F38">
-        <f ca="1">VLOOKUP($A38,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A38,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>15</v>
       </c>
       <c r="G38" t="str">
-        <f ca="1">VLOOKUP($A38,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A38,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>https://thefeedfeed.com/georgeats/green-halloumi-salad</v>
       </c>
     </row>
@@ -3983,27 +3983,27 @@
         <v>38</v>
       </c>
       <c r="B39" t="str">
-        <f ca="1">VLOOKUP($A39,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A39,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v/>
       </c>
       <c r="C39">
-        <f ca="1">VLOOKUP($A39,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A39,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>4</v>
       </c>
       <c r="D39">
-        <f ca="1">VLOOKUP($A39,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A39,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="E39">
-        <f ca="1">VLOOKUP($A39,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A39,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="F39" t="str">
-        <f ca="1">VLOOKUP($A39,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A39,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v/>
       </c>
       <c r="G39" t="str">
-        <f ca="1">VLOOKUP($A39,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A39,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v/>
       </c>
     </row>
@@ -4012,7 +4012,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="str">
-        <f ca="1">VLOOKUP($A40,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A40,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>1. Make the chimichurri by combining everything (cilantro, parsley, paprika, red onion, garlic, red wine vinegar, olive oil, salt, pepper) in a blender. It should be the consistency of a thick pourable sauce, so you may need to add a little more oil or a touch of hot water to thin it out.
 2. First, the hake: cut it into strips, then toss in a bowl with 1/4 cup chimichurri until fish is coated. Refrigerate for at least an hour and up to 3 hours.
 3. Toss the cabbage with a teaspoon or so of chimichurri, a drizzle of olive oil, and a pinch of salt. Set aside.
@@ -4022,23 +4022,23 @@
 7. Drizzle with the chimichurri crema, then garnish with onions, cilantro, and a squeeze of lime.</v>
       </c>
       <c r="C40">
-        <f ca="1">VLOOKUP($A40,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A40,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>4</v>
       </c>
       <c r="D40">
-        <f ca="1">VLOOKUP($A40,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A40,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="E40">
-        <f ca="1">VLOOKUP($A40,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A40,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="F40">
-        <f ca="1">VLOOKUP($A40,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A40,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>30</v>
       </c>
       <c r="G40" t="str">
-        <f ca="1">VLOOKUP($A40,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A40,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>https://camillestyles.com/food/the-chimichurri-fish-tacos-i-crave-all-summer/</v>
       </c>
     </row>
@@ -4047,7 +4047,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="str">
-        <f ca="1">VLOOKUP($A41,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A41,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>1. Toast sesame seeds.
 2. To make the slaw, combine CABBAGE, cooked QUINOA, CARROTS, CILANTRO, and GREEN ONIONS in a large mixing bowl. Cover and refrigerate until ready to dress and serve.
 3. To make the dressing, combine RICE VINEGAR, MAPLE SYRUP, SOY SAUCE, GINGER, and GARLIC in a mixing bowl. Slowly drizzle in OLIVE OIL and SESAME OIL, and whisk or blend until well-combined. Add SALT and PEPPER to taste.
@@ -4056,23 +4056,23 @@
 5. Store dressed slaw in an airtight container up to 24 hours. Non-dressed slaw can be stored up to 5 days.</v>
       </c>
       <c r="C41">
-        <f ca="1">VLOOKUP($A41,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A41,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>4</v>
       </c>
       <c r="D41">
-        <f ca="1">VLOOKUP($A41,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A41,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="E41">
-        <f ca="1">VLOOKUP($A41,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A41,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="F41">
-        <f ca="1">VLOOKUP($A41,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A41,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>20</v>
       </c>
       <c r="G41" t="str">
-        <f ca="1">VLOOKUP($A41,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A41,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>https://thekitchengirl.com/asian-quinoa-slaw-salad-sesame-ginger-vinaigrette/</v>
       </c>
     </row>
@@ -4081,27 +4081,27 @@
         <v>41</v>
       </c>
       <c r="B42" t="str">
-        <f ca="1">VLOOKUP($A42,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A42,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v/>
       </c>
       <c r="C42">
-        <f ca="1">VLOOKUP($A42,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A42,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>2</v>
       </c>
       <c r="D42">
-        <f ca="1">VLOOKUP($A42,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A42,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="E42">
-        <f ca="1">VLOOKUP($A42,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A42,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="F42" t="str">
-        <f ca="1">VLOOKUP($A42,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A42,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v/>
       </c>
       <c r="G42" t="str">
-        <f ca="1">VLOOKUP($A42,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A42,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>https://natashaskitchen.com/fish-tacos-recipe/</v>
       </c>
     </row>
@@ -4110,7 +4110,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="str">
-        <f ca="1">VLOOKUP($A43,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A43,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>1. Set a large soup pot over medium heat and pour in the olive oil. Swirl the oil around a bit and then add the onions to the pot and stir. The onions should be sizzling, but on the quieter end of sizzling. Lower the heat if necessary. Keep cooking the onions, stirring occasionally, until very soft and translucent (but not browning), about 7-8 minutes.
 2. Add the ground cumin and coriander to the pot, along with the ground chillies as well. Stir and cook along with the onions for one full minute.
 3. Then, add the minced garlic and ginger to the pot and stir. Keep cooking until the garlic is very fragrant, about 1 minute.
@@ -4123,23 +4123,23 @@
 10. Give the soup a taste at this point to see if you need to adjust some of the seasoning. Maybe it needs even more lemon/lime for your taste, some extra pepper etc. Adjust the seasoning to your liking and then serve! I topped mine with chopped cilantro, drizzles of tahini and chili oil, and sesame seeds.</v>
       </c>
       <c r="C43">
-        <f ca="1">VLOOKUP($A43,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A43,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>6</v>
       </c>
       <c r="D43">
-        <f ca="1">VLOOKUP($A43,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A43,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="E43">
-        <f ca="1">VLOOKUP($A43,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A43,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="F43">
-        <f ca="1">VLOOKUP($A43,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A43,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>65</v>
       </c>
       <c r="G43" t="str">
-        <f ca="1">VLOOKUP($A43,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A43,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>https://thefirstmess.com/2021/09/08/spicy-sesame-carrot-soup/#recipe</v>
       </c>
     </row>
@@ -4148,7 +4148,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="str">
-        <f ca="1">VLOOKUP($A44,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A44,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>This recipe is all about multi-tasking and is totally doable in 30 minutes.
 1. Start by preheating the oven to 218 C and cube your halloumi.
 2. Add halloumi to a medium mixing bowl. Season with curry powder, coconut aminos, sea salt, and nutritional yeast. Shake the bowl to gently toss. Set aside.
@@ -4165,23 +4165,23 @@
 Store leftovers covered in the refrigerator up to 4-5 days, or in the freezer up to 1 month. Reheat in the microwave or in a rimmed skillet until hot.</v>
       </c>
       <c r="C44">
-        <f ca="1">VLOOKUP($A44,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A44,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>4</v>
       </c>
       <c r="D44">
-        <f ca="1">VLOOKUP($A44,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A44,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="E44">
-        <f ca="1">VLOOKUP($A44,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A44,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="F44">
-        <f ca="1">VLOOKUP($A44,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A44,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>30</v>
       </c>
       <c r="G44" t="str">
-        <f ca="1">VLOOKUP($A44,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A44,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>https://minimalistbaker.com/vegan-palak-paneer-with-curried-tofu/</v>
       </c>
     </row>
@@ -4190,7 +4190,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="str">
-        <f ca="1">VLOOKUP($A45,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A45,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>1. Preheat the oven to 230°C fan.
 2. Place the sweetcorn in a large baking tray (with space for the seeds) with a drizzle of olive oil, a pinch of salt and the cumin. Mix well and cook for 15 minutes until crispy. Mix the sunflower seeds with the paprika, and add them to the corn for the last 5 minutes of the cooking time.
 3. While they cook, make the dressing and dip by placing the cashews in a food processor and pulsing until a smooth mixture forms - you may need to add a few tablespoons of the almond milk to help this along, it should take a minute or two. Once smooth, add the rest of the ingredients (1 avocado, lime juice, coriander, garlic), along with some salt, and pulse until smooth. You can add more almond milk depending on the consistency you like best.
@@ -4200,23 +4200,23 @@
 *you can add black beans to make this more filling</v>
       </c>
       <c r="C45">
-        <f ca="1">VLOOKUP($A45,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A45,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>4</v>
       </c>
       <c r="D45">
-        <f ca="1">VLOOKUP($A45,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A45,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="E45">
-        <f ca="1">VLOOKUP($A45,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A45,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="F45" t="str">
-        <f ca="1">VLOOKUP($A45,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A45,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v/>
       </c>
       <c r="G45" t="str">
-        <f ca="1">VLOOKUP($A45,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A45,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v/>
       </c>
     </row>
@@ -4225,7 +4225,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="str">
-        <f ca="1">VLOOKUP($A46,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A46,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>1. Put the onion and garlic into a saucepan over a medium heat with a drizzle of olive oil, a pinch of salt and pepper and gently heat for about 5 minutes, until softened. The smaller you've cut the onion the quicker it'll cook, and the better it will mix into the quinoa.
 2. Once the onion is soft, stir the quinoa into the mixture. Dissolve the stock cube in the boiling water then pour into the pan. Let the liquid come to the boil, then turn the heat down to a simmer and cook for 10-12 minutes, until the quinoa is light and fluffy.
 3. While the quinoa cooks, chop off the woody ends of the asparagus and slice the stems into rounds. Place in a frying pan with the courgette half-moons and a drizzle of olive oil and a pinch of salt and gently sauté on a medium heat, until soft.
@@ -4234,23 +4234,23 @@
 6. Add a handful of rocket and lots of pepper on the top of each serving.</v>
       </c>
       <c r="C46">
-        <f ca="1">VLOOKUP($A46,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A46,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>4</v>
       </c>
       <c r="D46">
-        <f ca="1">VLOOKUP($A46,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A46,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="E46">
-        <f ca="1">VLOOKUP($A46,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A46,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="F46">
-        <f ca="1">VLOOKUP($A46,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A46,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>30</v>
       </c>
       <c r="G46" t="str">
-        <f ca="1">VLOOKUP($A46,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A46,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v/>
       </c>
     </row>
@@ -4259,7 +4259,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="str">
-        <f ca="1">VLOOKUP($A47,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A47,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>1. Rinse quinoa well and place it in a small pot that you have a glass lid for. Add a few pinches of salt and 180 ml / ¾ cup of water, cover with a lid and bring to the boil. Once the water boils, decrease the heat to low-medium and let the quinoa simmer until all the water has been absorbed. To check, tilt the pot slightly, keeping the lid firmly on. If you see no water seeping out from under the grain, switch off the heat and let the quinoa sit (with the lid firmly on) for another 5-10 min to finish off cooking in its own steam. Cool it down completely.
 2. Divide broccoli into small florets, snap wooden ends off the asparagus and cut zucchini into 0.5 cm / ¼” slices.
 3. ROAST: Preheat the oven to 220° C / 428° F. Coat broccoli florets in 2 tsp of olive oil and season. Arrange on a large baking tray. Brush zucchini slices with olive oil on both sides, season and arrange on the same tray. Coat asparagus spears in 1 tsp of oil, season and place on the baking tray. Roast for about 8 minutes, take the asparagus off the tray if ready, carry on roasting broccoli and zucchini for another 5-7 minutes, until cooked through. Alternatively, you could use a griddle pan if you prefer.
@@ -4270,23 +4270,23 @@
 8. Arrange all of the salad elements on a large platter, dress with approximately half of the dressing (keep the rest in the fridge, use up in the next few days) and sprinkle with toasted almonds at the end. Pieces of soft vegan cheese, like this almond feta, scattered on top are also a nice addition.</v>
       </c>
       <c r="C47">
-        <f ca="1">VLOOKUP($A47,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A47,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>4</v>
       </c>
       <c r="D47">
-        <f ca="1">VLOOKUP($A47,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A47,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="E47">
-        <f ca="1">VLOOKUP($A47,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A47,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="F47">
-        <f ca="1">VLOOKUP($A47,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A47,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>40</v>
       </c>
       <c r="G47" t="str">
-        <f ca="1">VLOOKUP($A47,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A47,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>https://www.lazycatkitchen.com/green-vegan-salad/#recipe-start</v>
       </c>
     </row>
@@ -4295,7 +4295,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="str">
-        <f ca="1">VLOOKUP($A48,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A48,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>1. Heat a large, heavy-bottomed soup pot over medium heat. Add the coconut oil to the pot and let it melt. Add the onions
 to the pot and stir. Saute the onions, stirring occasionally,
 until translucent and quite soft, about 5 minutes. Add the chili flakes, coriander, cumin, and turmeric. Saute spices until very fragrant, about 1 minute. Add the ginger and garlic to
@@ -4307,23 +4307,23 @@
 5. Serve the sweet potato and coconut milk stew hot with chopped cilantro, extra chili flakes, lime wedges, and Nigella seeds (if using).</v>
       </c>
       <c r="C48">
-        <f ca="1">VLOOKUP($A48,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A48,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>6</v>
       </c>
       <c r="D48">
-        <f ca="1">VLOOKUP($A48,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A48,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="E48">
-        <f ca="1">VLOOKUP($A48,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A48,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="F48">
-        <f ca="1">VLOOKUP($A48,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A48,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>65</v>
       </c>
       <c r="G48" t="str">
-        <f ca="1">VLOOKUP($A48,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A48,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>https://thefirstmess.com/2020/02/19/sweet-potato-coconut-milk-stew/#recipe</v>
       </c>
     </row>
@@ -4332,7 +4332,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="str">
-        <f ca="1">VLOOKUP($A49,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A49,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>Preheat the oven to 180C/gas mark 4.
 Combine the oat and almond flours, cornflour and sea salt in a bowl.
 Add the coconut oil and ice-cold water.
@@ -4356,23 +4356,23 @@
 Let it cool for a while before serving.</v>
       </c>
       <c r="C49">
-        <f ca="1">VLOOKUP($A49,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A49,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>4</v>
       </c>
       <c r="D49">
-        <f ca="1">VLOOKUP($A49,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A49,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="E49">
-        <f ca="1">VLOOKUP($A49,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A49,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="F49">
-        <f ca="1">VLOOKUP($A49,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A49,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>45</v>
       </c>
       <c r="G49" t="str">
-        <f ca="1">VLOOKUP($A49,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A49,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>https://www.google.com/amp/s/greenkitchenstories.com/feta-spinach-pie-with-an-oat-crust/%3Famp</v>
       </c>
     </row>
@@ -4381,7 +4381,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="str">
-        <f ca="1">VLOOKUP($A50,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A50,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>1 Slice into the brinjals, leaving the tops still intact, to make a fan shape.
 2 Heat a large pan and add half the olive oil. Fry the brinjals until golden brown on both sides, seasoning with salt and pepper. Place in an ovenproof dish.
 3 Preheat the oven to 200°C. To make the sauce, heat a saucepan and add the remaining olive oil. Fry the onion over a medium heat until it begins to soften and caramelise slightly.
@@ -4389,23 +4389,23 @@
 5 Simmer for 10 minutes, then pour over the brinjals. Crumble over the feta, top with the mozzarella and cover with tinfoil. Bake for 20 minutes, or until the brinjals are soft and cooked through when pierced with a knife. Uncover and grill until golden brown. To serve, spoon over the basil pesto and top with torn basil leaves.</v>
       </c>
       <c r="C50">
-        <f ca="1">VLOOKUP($A50,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A50,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>6</v>
       </c>
       <c r="D50">
-        <f ca="1">VLOOKUP($A50,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A50,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="E50">
-        <f ca="1">VLOOKUP($A50,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A50,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="F50">
-        <f ca="1">VLOOKUP($A50,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A50,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>40</v>
       </c>
       <c r="G50" t="str">
-        <f ca="1">VLOOKUP($A50,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A50,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>https://taste.co.za/recipes/cheesy-brinjal-bake/</v>
       </c>
     </row>
@@ -4414,7 +4414,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="str">
-        <f ca="1">VLOOKUP($A51,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A51,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>1. Preheat oven to 200C.
 2. Cut butternut into roughly equal sized cubes about 1/2-1 inch.
 3. Place on a large baking tray, drizzle generously with oil salt and pepper, toss and place in the oven for 35-40 minutes until soft through and starting to brown on the edges.
@@ -4425,23 +4425,23 @@
 8. Add the roasted butternut squash, stir and serve! Top with some chopped fresh coriander and serve with basmati rice and your favourite sides - like my onion bhajis!</v>
       </c>
       <c r="C51">
-        <f ca="1">VLOOKUP($A51,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A51,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>4</v>
       </c>
       <c r="D51">
-        <f ca="1">VLOOKUP($A51,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A51,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="E51">
-        <f ca="1">VLOOKUP($A51,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A51,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="F51">
-        <f ca="1">VLOOKUP($A51,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A51,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>55</v>
       </c>
       <c r="G51" t="str">
-        <f ca="1">VLOOKUP($A51,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A51,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>https://cupfulofkale.com/vegan-roasted-butternut-squash-and-chickpea-curry/</v>
       </c>
     </row>
@@ -4450,7 +4450,7 @@
         <v>51</v>
       </c>
       <c r="B52" t="str">
-        <f ca="1">VLOOKUP($A52,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A52,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>Wash all the produce.
 Peel and chop the onion and carrot(s).
 De-stem, de-seed and chop the pepper.
@@ -4475,23 +4475,23 @@
 The chili will keep in the refrigerator for up to 4 days, or you can freeze for up to one month.</v>
       </c>
       <c r="C52">
-        <f ca="1">VLOOKUP($A52,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A52,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>4</v>
       </c>
       <c r="D52">
-        <f ca="1">VLOOKUP($A52,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A52,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="E52">
-        <f ca="1">VLOOKUP($A52,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A52,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="F52" t="str">
-        <f ca="1">VLOOKUP($A52,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A52,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v/>
       </c>
       <c r="G52" t="str">
-        <f ca="1">VLOOKUP($A52,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A52,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>https://mymeals.earthyandy.com/recipe/6025ce03b6c8c2e513dae502</v>
       </c>
     </row>
@@ -4500,7 +4500,7 @@
         <v>52</v>
       </c>
       <c r="B53" t="str">
-        <f ca="1">VLOOKUP($A53,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A53,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>In an upright, high speed blender, combine the drained cashews, water, and maple syrup. Blend on high until you have a heavy cream-like consistency, about 1 minute. Set aside.
 Place a large, deep skillet (or braiser) over medium heat.
 Add the coconut oil to the skillet and swirl it around.
@@ -4520,23 +4520,23 @@
 Serve hot with rice or flatbread of choice.</v>
       </c>
       <c r="C53">
-        <f ca="1">VLOOKUP($A53,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A53,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>4</v>
       </c>
       <c r="D53">
-        <f ca="1">VLOOKUP($A53,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A53,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="E53">
-        <f ca="1">VLOOKUP($A53,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A53,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="F53">
-        <f ca="1">VLOOKUP($A53,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A53,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>40</v>
       </c>
       <c r="G53" t="str">
-        <f ca="1">VLOOKUP($A53,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A53,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>https://thefirstmess.com/2019/09/11/spiced-vegan-butter-chickpeas/</v>
       </c>
     </row>
@@ -4545,7 +4545,7 @@
         <v>53</v>
       </c>
       <c r="B54" t="str">
-        <f ca="1">VLOOKUP($A54,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A54,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>Preheat the oven to 190C, fan setting.
 Cut the butternut squash in half widthways.
 Scrape out the seeds from one side before cutting
@@ -4572,23 +4572,23 @@
 serving.</v>
       </c>
       <c r="C54">
-        <f ca="1">VLOOKUP($A54,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A54,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>4</v>
       </c>
       <c r="D54">
-        <f ca="1">VLOOKUP($A54,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A54,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="E54">
-        <f ca="1">VLOOKUP($A54,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A54,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="F54">
-        <f ca="1">VLOOKUP($A54,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A54,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>35</v>
       </c>
       <c r="G54" t="str">
-        <f ca="1">VLOOKUP($A54,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A54,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v/>
       </c>
     </row>
@@ -4597,7 +4597,7 @@
         <v>54</v>
       </c>
       <c r="B55" t="str">
-        <f ca="1">VLOOKUP($A55,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A55,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>Firstly add all the sauce ingredients into a
 blender and whizz into a smooth sauce
 Now heat a wok/pan/pot with coconut oil + tamari
@@ -4607,23 +4607,23 @@
 fresh coriander.</v>
       </c>
       <c r="C55">
-        <f ca="1">VLOOKUP($A55,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A55,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>4</v>
       </c>
       <c r="D55">
-        <f ca="1">VLOOKUP($A55,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A55,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="E55">
-        <f ca="1">VLOOKUP($A55,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A55,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="F55">
-        <f ca="1">VLOOKUP($A55,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A55,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>30</v>
       </c>
       <c r="G55" t="str">
-        <f ca="1">VLOOKUP($A55,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A55,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v/>
       </c>
     </row>
@@ -4632,27 +4632,27 @@
         <v>55</v>
       </c>
       <c r="B56" t="str">
-        <f ca="1">VLOOKUP($A56,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A56,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v/>
       </c>
       <c r="C56" t="str">
-        <f ca="1">VLOOKUP($A56,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A56,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v/>
       </c>
       <c r="D56">
-        <f ca="1">VLOOKUP($A56,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A56,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="E56">
-        <f ca="1">VLOOKUP($A56,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A56,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="F56" t="str">
-        <f ca="1">VLOOKUP($A56,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A56,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v/>
       </c>
       <c r="G56" t="str">
-        <f ca="1">VLOOKUP($A56,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A56,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>https://www.servingdumplings.com/recipes/thai-coconut-shrimp-curry/</v>
       </c>
     </row>
@@ -4661,7 +4661,7 @@
         <v>56</v>
       </c>
       <c r="B57" t="str">
-        <f ca="1">VLOOKUP($A57,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A57,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>Mash bananas.
 Beat eggs.
 Combine all ingredients.
@@ -4669,23 +4669,23 @@
 Serve with yoghurt and peaches.</v>
       </c>
       <c r="C57" t="str">
-        <f ca="1">VLOOKUP($A57,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A57,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v/>
       </c>
       <c r="D57">
-        <f ca="1">VLOOKUP($A57,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A57,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="E57">
-        <f ca="1">VLOOKUP($A57,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A57,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="F57" t="str">
-        <f ca="1">VLOOKUP($A57,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A57,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v/>
       </c>
       <c r="G57" t="str">
-        <f ca="1">VLOOKUP($A57,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A57,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v/>
       </c>
     </row>
@@ -4694,7 +4694,7 @@
         <v>57</v>
       </c>
       <c r="B58" t="str">
-        <f ca="1">VLOOKUP($A58,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A58,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>1. Add all the ingredients to a food processor and pulse until combined.
 2. Scoop out some dough using a spoon and roll into balls. 
 3. Roll each ball into the shredded coconut to coat. 
@@ -4702,23 +4702,23 @@
 Store these energy balls in the fridge for up to 2 weeks.</v>
       </c>
       <c r="C58">
-        <f ca="1">VLOOKUP($A58,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A58,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>12</v>
       </c>
       <c r="D58">
-        <f ca="1">VLOOKUP($A58,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A58,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="E58">
-        <f ca="1">VLOOKUP($A58,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A58,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="F58">
-        <f ca="1">VLOOKUP($A58,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A58,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>15</v>
       </c>
       <c r="G58" t="str">
-        <f ca="1">VLOOKUP($A58,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A58,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>https://choosingchia.com/carrot-cake-energy-balls/</v>
       </c>
     </row>
@@ -4727,7 +4727,7 @@
         <v>58</v>
       </c>
       <c r="B59" t="str">
-        <f ca="1">VLOOKUP($A59,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A59,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>1. Thoroughly rinse one 15oz can of chickpeas in a strainer. Pat the chickpeas dry using a towel.
 2. Add the chickpeas to a bowl. To the bowl, add 1 tsp melted coconut oil. Mix the contents of the bowl until the chickpeas are evenly coated.
 3. Evenly space the chickpeas across a baking dish. Bake at 400 degrees for about 30 minutes or until the chickpeas are crispy. Alternatively, air fry the chickpeas at 400 degrees for about 20-25 minutes or until the chickpeas are crispy. Remove the chickpeas from the oven and allow them to cool.
@@ -4736,23 +4736,23 @@
 6. Once hardened, remove the chocolate from the bread pan and cut into bars.</v>
       </c>
       <c r="C59" t="str">
-        <f ca="1">VLOOKUP($A59,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A59,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v/>
       </c>
       <c r="D59">
-        <f ca="1">VLOOKUP($A59,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A59,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="E59">
-        <f ca="1">VLOOKUP($A59,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A59,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="F59">
-        <f ca="1">VLOOKUP($A59,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A59,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>35</v>
       </c>
       <c r="G59" t="str">
-        <f ca="1">VLOOKUP($A59,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A59,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>https://wellbymelnutrition.com/chickpea-crunch-bars/</v>
       </c>
     </row>
@@ -4761,30 +4761,30 @@
         <v>59</v>
       </c>
       <c r="B60" t="str">
-        <f ca="1">VLOOKUP($A60,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A60,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>In a small saucepan, bring the coconut milk, maple syrup and vanilla extract to a boil. Cover and simmer for 20 minutes (or until mixture is golden brown and starts to thicken), stirring every few minutes. The mixture does not need to be thick like caramel for this recipe! 
 Combine the caramel mixture with almond butter. Line a bread pan with parchment paper &amp; pour mixture evenly across bottom.
 Freeze for 2-3 hours or until filling is hard enough to cut into squares. 
 Cut into 24-30 small squares. Place back in the freezer while you melt the chocolate. Using a fork, dip each square in the melted chocolate and place on a baking sheet lined with parchment paper. Sprinkle with sea salt and place back in the freezer for ~1 hour.</v>
       </c>
       <c r="C60" t="str">
-        <f ca="1">VLOOKUP($A60,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A60,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v/>
       </c>
       <c r="D60">
-        <f ca="1">VLOOKUP($A60,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A60,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="E60">
-        <f ca="1">VLOOKUP($A60,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A60,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="F60" t="str">
-        <f ca="1">VLOOKUP($A60,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A60,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v/>
       </c>
       <c r="G60" t="str">
-        <f ca="1">VLOOKUP($A60,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A60,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>https://figgindelicious.com/salted-caramel-almond-butter-bites/</v>
       </c>
     </row>
@@ -4793,29 +4793,29 @@
         <v>60</v>
       </c>
       <c r="B61" t="str">
-        <f ca="1">VLOOKUP($A61,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A61,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>1. Mix the flour and chia seeds in a large bowl. Then add the almond milk, melted coconut oil and maple syrup; mix well, until a smooth batter forms. Set the batter aside for 4-5 minutes to thicken a little.
 2. Next, warm some coconut oil in a pan over medium heat. Once the pan is hot, add a large spoonful of batter to the pan, moving the pan around (it needed) to make a pancake shape.
 3. As the pancake begins to set, sprinkle some fresh blueberries on top and cook for 3-5 minutes, until the bottom feels cooked. Flip and cook on the other side, until cooked through.</v>
       </c>
       <c r="C61" t="str">
-        <f ca="1">VLOOKUP($A61,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A61,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v/>
       </c>
       <c r="D61">
-        <f ca="1">VLOOKUP($A61,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A61,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="E61">
-        <f ca="1">VLOOKUP($A61,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A61,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="F61" t="str">
-        <f ca="1">VLOOKUP($A61,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A61,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v/>
       </c>
       <c r="G61" t="str">
-        <f ca="1">VLOOKUP($A61,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A61,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v/>
       </c>
     </row>
@@ -4824,30 +4824,30 @@
         <v>61</v>
       </c>
       <c r="B62" t="str">
-        <f ca="1">VLOOKUP($A62,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A62,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>1. Drain, rinse and dry the chickpeas.
 2. Roast at 220 degree Celsius for 30 mins.
 3. Blend with other ingredients (hot water).
 4. Store in the fridge.</v>
       </c>
       <c r="C62">
-        <f ca="1">VLOOKUP($A62,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A62,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>10</v>
       </c>
       <c r="D62">
-        <f ca="1">VLOOKUP($A62,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A62,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="E62">
-        <f ca="1">VLOOKUP($A62,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A62,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="F62" t="str">
-        <f ca="1">VLOOKUP($A62,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A62,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v/>
       </c>
       <c r="G62" t="str">
-        <f ca="1">VLOOKUP($A62,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A62,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v/>
       </c>
     </row>
@@ -4856,30 +4856,30 @@
         <v>62</v>
       </c>
       <c r="B63" t="str">
-        <f ca="1">VLOOKUP($A63,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A63,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>1. Cute bananas lengthways.
 2. Put peanut butter on the banana.
 3. Sprinkle peanuts over the banana.
 4. Drizzle over chocolate.</v>
       </c>
       <c r="C63" t="str">
-        <f ca="1">VLOOKUP($A63,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A63,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v/>
       </c>
       <c r="D63">
-        <f ca="1">VLOOKUP($A63,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A63,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="E63">
-        <f ca="1">VLOOKUP($A63,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A63,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="F63" t="str">
-        <f ca="1">VLOOKUP($A63,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A63,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v/>
       </c>
       <c r="G63" t="str">
-        <f ca="1">VLOOKUP($A63,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A63,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v/>
       </c>
     </row>
@@ -4888,29 +4888,29 @@
         <v>63</v>
       </c>
       <c r="B64" t="str">
-        <f ca="1">VLOOKUP($A64,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A64,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>1. Freeze bananas.
 2. Cool coconut milk.
 3. Blend all ingredients.</v>
       </c>
       <c r="C64">
-        <f ca="1">VLOOKUP($A64,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A64,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>2</v>
       </c>
       <c r="D64">
-        <f ca="1">VLOOKUP($A64,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A64,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="E64">
-        <f ca="1">VLOOKUP($A64,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A64,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="F64" t="str">
-        <f ca="1">VLOOKUP($A64,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A64,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v/>
       </c>
       <c r="G64" t="str">
-        <f ca="1">VLOOKUP($A64,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A64,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>https://www.instagram.com/p/CLjCbRfpkH0/</v>
       </c>
     </row>
@@ -4919,7 +4919,7 @@
         <v>64</v>
       </c>
       <c r="B65" t="str">
-        <f ca="1">VLOOKUP($A65,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A65,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>Brown the butter over medium heat, stirring constantly until the butter begins to foam and turns a golden brown, emitting a nutty aroma. Make sure you only brown the butter lightly. When butter browns the liquid evaporates off which can dry out your dough. As soon as the butter starts to turn brown and smell nutty, take it off the heat to prevent any more liquid from escaping.  Take butter off the heat and allow to cool.
 In a large mixing bowl combine the cooled brown butter, brown sugar, and white sugar. Beat until mixed together. Add in the egg, egg yolk, and vanilla extract. Mix well.
 In separate bowl mix together the flour, salt and baking soda. Mix half the dry ingredients into the wet until everything comes together. Slowly add in the remaining flour a little bit at a time, stopping if the dough starts to get too dry.* Fold in the chocolate. Do not over mix.
@@ -4928,23 +4928,23 @@
 Allow to cool before eating!</v>
       </c>
       <c r="C65">
-        <f ca="1">VLOOKUP($A65,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A65,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>16</v>
       </c>
       <c r="D65">
-        <f ca="1">VLOOKUP($A65,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A65,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="E65">
-        <f ca="1">VLOOKUP($A65,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A65,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="F65" t="str">
-        <f ca="1">VLOOKUP($A65,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A65,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v/>
       </c>
       <c r="G65" t="str">
-        <f ca="1">VLOOKUP($A65,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A65,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>https://bromabakery.com/best-chocolate-chip-cookies/</v>
       </c>
     </row>
@@ -4953,7 +4953,7 @@
         <v>65</v>
       </c>
       <c r="B66" t="str">
-        <f ca="1">VLOOKUP($A66,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A66,[1]Sheet8!$B:$H,MATCH([1]recipes!B$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>1. Preheat the oven to 200°C and line a baking tray with baking paper.
 2. Coarsely chop the broccoli (use the brighter part of the stem too), place in food processor and blend until you have got a fine rice-like texture.
 3. Measure 4 cups of the vegetable ‘rice’ and place in a mixing bowl.
@@ -4968,23 +4968,23 @@
 12. Cut into bread-sized slices and store in the fridge.</v>
       </c>
       <c r="C66">
-        <f ca="1">VLOOKUP($A66,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A66,[1]Sheet8!$B:$H,MATCH([1]recipes!C$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>12</v>
       </c>
       <c r="D66">
-        <f ca="1">VLOOKUP($A66,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A66,[1]Sheet8!$B:$H,MATCH([1]recipes!D$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="E66">
-        <f ca="1">VLOOKUP($A66,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A66,[1]Sheet8!$B:$H,MATCH([1]recipes!E$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>0</v>
       </c>
       <c r="F66">
-        <f ca="1">VLOOKUP($A66,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A66,[1]Sheet8!$B:$H,MATCH([1]recipes!F$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>45</v>
       </c>
       <c r="G66" t="str">
-        <f ca="1">VLOOKUP($A66,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
+        <f>VLOOKUP($A66,[1]Sheet8!$B:$H,MATCH([1]recipes!G$1,[1]Sheet8!$B$1:$H$1,0),0)</f>
         <v>https://greenkitchenstories.com/vegetable-flatbreads/</v>
       </c>
     </row>

</xml_diff>